<commit_message>
Copycat completed and Suppression attack started'
</commit_message>
<xml_diff>
--- a/examples/ipv6/suppression-attack/CopyCat/random_seed_list.xlsx
+++ b/examples/ipv6/suppression-attack/CopyCat/random_seed_list.xlsx
@@ -54,7 +54,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -65,6 +65,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF200"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC2E0AE"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -108,7 +114,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -117,11 +123,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -150,7 +160,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFC2E0AE"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -202,10 +212,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -221,24 +231,33 @@
       <c r="D1" s="1" t="n">
         <v>123456</v>
       </c>
+      <c r="F1" s="2" t="n">
+        <v>765765</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>487575</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>495363</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>293847</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>427044</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="4" t="n">
         <v>427044</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>124856</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>876976</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -248,13 +267,19 @@
       <c r="D4" s="1" t="n">
         <v>124897</v>
       </c>
+      <c r="F4" s="2" t="n">
+        <v>124897</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="4" t="n">
         <v>691856</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>169859</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>111685</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -264,6 +289,9 @@
       <c r="D6" s="1" t="n">
         <v>154258</v>
       </c>
+      <c r="F6" s="2" t="n">
+        <v>549849</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -272,6 +300,9 @@
       <c r="D7" s="1" t="n">
         <v>155458</v>
       </c>
+      <c r="F7" s="2" t="n">
+        <v>686986</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -280,6 +311,9 @@
       <c r="D8" s="1" t="n">
         <v>124785</v>
       </c>
+      <c r="F8" s="2" t="n">
+        <v>979845</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -288,6 +322,9 @@
       <c r="D9" s="1" t="n">
         <v>125484</v>
       </c>
+      <c r="F9" s="2" t="n">
+        <v>916619</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -295,6 +332,9 @@
       </c>
       <c r="D10" s="1" t="n">
         <v>125499</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>398097</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>